<commit_message>
çalışıyo ama excelcs 118. satır sorunlu bi geri dönücem
</commit_message>
<xml_diff>
--- a/Zil/Zil/zil.xlsx
+++ b/Zil/Zil/zil.xlsx
@@ -221,12 +221,12 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="91.42"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
zil % test any %
</commit_message>
<xml_diff>
--- a/Zil/Zil/zil.xlsx
+++ b/Zil/Zil/zil.xlsx
@@ -52,7 +52,7 @@
     <t xml:space="preserve">der1</t>
   </si>
   <si>
-    <t xml:space="preserve">15.37</t>
+    <t xml:space="preserve">14.59</t>
   </si>
   <si>
     <t xml:space="preserve">10*3</t>
@@ -221,10 +221,10 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="91.42"/>

</xml_diff>